<commit_message>
apresentacao do projeto final
</commit_message>
<xml_diff>
--- a/analise_da_evasao_estudantil/Docs Complementares/quadro_grupos_cotas.xlsx
+++ b/analise_da_evasao_estudantil/Docs Complementares/quadro_grupos_cotas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alinefonseca/Dropbox/Mac/Documents/GitHub/projetos-do-bootcamp-analise-de-dados-enap-2023/analise_da_evasao_estudantil/Docs Complementares/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92ED1570-EC30-FA47-9EF5-95DBF1E101D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2160E9B1-50B1-1A4C-BEF6-20214C5BDF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16840" xr2:uid="{B7917D34-F753-CB40-8D7F-2C5CF3295AA0}"/>
   </bookViews>
@@ -98,15 +98,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -114,12 +126,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +467,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,169 +479,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>